<commit_message>
Remove spacial characters from UC_N
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Demand.xlsx
+++ b/SuppXLS/Scen_TRA_Demand.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\VA_Transport\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C597AB4B-B55E-46D6-9DCE-1EE65F8A48A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE68E59-C47A-4B3A-B58E-20F0A0701684}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INS" sheetId="2" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="96">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -351,9 +351,6 @@
     <t>THRAIL*</t>
   </si>
   <si>
-    <t>UC_walking-S</t>
-  </si>
-  <si>
     <t>UC_cycling_S</t>
   </si>
   <si>
@@ -367,9 +364,6 @@
   </si>
   <si>
     <t>UC_BUS_S</t>
-  </si>
-  <si>
-    <t>UC_Light rail (LUAS)_S</t>
   </si>
   <si>
     <t>UC_Train_S</t>
@@ -393,9 +387,6 @@
     <t>UC_BUS_M</t>
   </si>
   <si>
-    <t>UC_Light rail (LUAS)_M</t>
-  </si>
-  <si>
     <t>UC_Train_M</t>
   </si>
   <si>
@@ -417,10 +408,13 @@
     <t>UC_BUS_L</t>
   </si>
   <si>
-    <t>UC_Light rail (LUAS)_L</t>
+    <t>UC_Train_L</t>
   </si>
   <si>
-    <t>UC_Train_L</t>
+    <t>UC_Light_rail_LUAS_S</t>
+  </si>
+  <si>
+    <t>UC_walking_S</t>
   </si>
 </sst>
 </file>
@@ -3960,30 +3954,30 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="34" width="10.6640625" customWidth="1"/>
     <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.53125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
       <c r="B2" s="9" t="s">
         <v>16</v>
       </c>
@@ -3996,7 +3990,7 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
@@ -4133,30 +4127,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="34" width="10.6640625" customWidth="1"/>
     <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.53125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
       <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
@@ -4169,7 +4163,7 @@
       <c r="AO2" s="11"/>
       <c r="AP2" s="11"/>
     </row>
-    <row r="3" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
@@ -4305,37 +4299,37 @@
   <dimension ref="B6:AO53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.796875" customWidth="1"/>
+    <col min="14" max="14" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:41" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C7" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:41" x14ac:dyDescent="0.45">
       <c r="K9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C10" s="28" t="s">
         <v>1</v>
       </c>
@@ -4481,9 +4475,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="E11" t="str">
         <f>[1]Commodities!$K$8</f>
@@ -4618,9 +4612,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E12" t="str">
         <f>[1]Commodities!$K$9</f>
@@ -4755,9 +4749,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" t="str">
         <f>[1]Commodities!$K$11</f>
@@ -4892,9 +4886,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
         <v>71</v>
@@ -5028,9 +5022,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
         <v>72</v>
@@ -5164,9 +5158,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:41" x14ac:dyDescent="0.45">
       <c r="C16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" t="str">
         <f>[1]Commodities!$K$27</f>
@@ -5301,9 +5295,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C17" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="E17" t="str">
         <f>[1]Commodities!$K$29</f>
@@ -5438,9 +5432,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C18" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D18" s="32"/>
       <c r="E18" s="32" t="s">
@@ -5578,27 +5572,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:41" x14ac:dyDescent="0.45">
       <c r="N19" s="31"/>
     </row>
-    <row r="20" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:41" x14ac:dyDescent="0.45">
       <c r="N20" s="31"/>
     </row>
-    <row r="21" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:41" x14ac:dyDescent="0.45">
       <c r="N21" s="31"/>
     </row>
-    <row r="24" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C25" s="7"/>
     </row>
-    <row r="26" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:41" x14ac:dyDescent="0.45">
       <c r="K26" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C27" s="28" t="s">
         <v>1</v>
       </c>
@@ -5744,9 +5738,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E28" t="str">
         <f>[1]Commodities!$K$8</f>
@@ -5882,9 +5876,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E29" t="str">
         <f>[1]Commodities!$K$9</f>
@@ -6020,9 +6014,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C30" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E30" t="str">
         <f>[1]Commodities!$K$11</f>
@@ -6158,9 +6152,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C31" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E31" t="s">
         <v>71</v>
@@ -6295,9 +6289,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E32" t="s">
         <v>72</v>
@@ -6432,9 +6426,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E33" t="str">
         <f>[1]Commodities!$K$27</f>
@@ -6570,9 +6564,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C34" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E34" t="str">
         <f>[1]Commodities!$K$29</f>
@@ -6708,9 +6702,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C35" s="32" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D35" s="32"/>
       <c r="E35" s="32" t="s">
@@ -6849,13 +6843,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C43" s="7"/>
     </row>
-    <row r="44" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C44" s="34"/>
       <c r="D44" s="34"/>
       <c r="E44" s="34"/>
@@ -6898,7 +6892,7 @@
       <c r="AN44" s="34"/>
       <c r="AO44" s="34"/>
     </row>
-    <row r="45" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C45" s="5" t="s">
         <v>1</v>
       </c>
@@ -7044,9 +7038,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C46" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D46" s="34"/>
       <c r="E46" s="34" t="str">
@@ -7186,9 +7180,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C47" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D47" s="34"/>
       <c r="E47" s="34" t="str">
@@ -7328,9 +7322,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C48" s="34" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D48" s="34"/>
       <c r="E48" s="34" t="str">
@@ -7470,9 +7464,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C49" s="34" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D49" s="34"/>
       <c r="E49" s="34" t="s">
@@ -7611,9 +7605,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C50" s="34" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D50" s="34"/>
       <c r="E50" s="34" t="s">
@@ -7752,9 +7746,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C51" s="34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D51" s="34"/>
       <c r="E51" s="34" t="str">
@@ -7894,9 +7888,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:41" x14ac:dyDescent="0.3">
-      <c r="C52" s="34" t="s">
-        <v>96</v>
+    <row r="52" spans="3:41" x14ac:dyDescent="0.45">
+      <c r="C52" t="s">
+        <v>94</v>
       </c>
       <c r="D52" s="34"/>
       <c r="E52" s="34" t="str">
@@ -8036,9 +8030,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:41" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:41" x14ac:dyDescent="0.45">
       <c r="C53" s="32" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D53" s="32"/>
       <c r="E53" s="32" t="s">
@@ -8189,33 +8183,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -8273,33 +8267,33 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.53125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -8355,32 +8349,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="13" max="13" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B3" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="J4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -8438,12 +8432,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>16</v>
       </c>
@@ -8478,7 +8472,7 @@
       <c r="AF2" s="15"/>
       <c r="AG2" s="15"/>
     </row>
-    <row r="3" spans="2:33" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:33" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="17" t="s">
         <v>17</v>
       </c>
@@ -8603,7 +8597,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B4" s="15"/>
       <c r="C4" s="15"/>
       <c r="D4" s="15" t="s">
@@ -8724,7 +8718,7 @@
         <v>0.20769618859639608</v>
       </c>
     </row>
-    <row r="5" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:33" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15" t="s">
@@ -8845,7 +8839,7 @@
         <v>0.2284658074560357</v>
       </c>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15" t="s">
@@ -8966,7 +8960,7 @@
         <v>0.47664625412085693</v>
       </c>
     </row>
-    <row r="7" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:33" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15" t="s">
@@ -9087,7 +9081,7 @@
         <v>0.52431087953294264</v>
       </c>
     </row>
-    <row r="8" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15" t="s">
@@ -9208,7 +9202,7 @@
         <v>0.42809298937083867</v>
       </c>
     </row>
-    <row r="9" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:33" ht="15.75" x14ac:dyDescent="0.5">
       <c r="B9" s="22"/>
       <c r="C9" s="22"/>
       <c r="D9" s="22" t="s">
@@ -9329,29 +9323,29 @@
         <v>0.47090228830792258</v>
       </c>
     </row>
-    <row r="10" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
     </row>
-    <row r="11" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B11" s="15"/>
       <c r="C11" s="15"/>
       <c r="D11" s="15"/>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B12" s="15"/>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B13" s="15" t="s">
         <v>63</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B14" s="15" t="s">
         <v>64</v>
       </c>
@@ -9362,7 +9356,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B15" s="15" t="s">
         <v>65</v>
       </c>
@@ -9373,7 +9367,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B16" s="15" t="s">
         <v>66</v>
       </c>
@@ -9384,7 +9378,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B17" s="15" t="s">
         <v>67</v>
       </c>
@@ -9395,137 +9389,137 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
       <c r="D18" s="15"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B19" s="15"/>
       <c r="C19" s="15"/>
       <c r="D19" s="15"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B22" s="15"/>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15"/>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15"/>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D38" s="15"/>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D40" s="15"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D41" s="15"/>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D42" s="15"/>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D43" s="15"/>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D44" s="15"/>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D45" s="15"/>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D46" s="15"/>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.45">
       <c r="D47" s="15"/>
     </row>
-    <row r="52" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="52" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
       <c r="G52" s="15"/>
@@ -9556,7 +9550,7 @@
       <c r="AF52" s="15"/>
       <c r="AG52" s="15"/>
     </row>
-    <row r="53" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="53" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E53" s="15"/>
       <c r="F53" s="15"/>
       <c r="G53" s="15"/>
@@ -9587,7 +9581,7 @@
       <c r="AF53" s="15"/>
       <c r="AG53" s="15"/>
     </row>
-    <row r="54" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="54" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E54" s="15"/>
       <c r="F54" s="15"/>
       <c r="G54" s="15"/>
@@ -9618,7 +9612,7 @@
       <c r="AF54" s="15"/>
       <c r="AG54" s="15"/>
     </row>
-    <row r="55" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="55" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E55" s="15"/>
       <c r="F55" s="15"/>
       <c r="G55" s="15"/>
@@ -9649,7 +9643,7 @@
       <c r="AF55" s="15"/>
       <c r="AG55" s="15"/>
     </row>
-    <row r="56" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="56" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E56" s="15"/>
       <c r="F56" s="15"/>
       <c r="G56" s="15"/>
@@ -9680,7 +9674,7 @@
       <c r="AF56" s="15"/>
       <c r="AG56" s="15"/>
     </row>
-    <row r="57" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="57" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E57" s="15"/>
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
@@ -9711,7 +9705,7 @@
       <c r="AF57" s="15"/>
       <c r="AG57" s="15"/>
     </row>
-    <row r="58" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="58" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E58" s="15"/>
       <c r="F58" s="15"/>
       <c r="G58" s="15"/>
@@ -9742,7 +9736,7 @@
       <c r="AF58" s="15"/>
       <c r="AG58" s="15"/>
     </row>
-    <row r="59" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="59" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E59" s="15"/>
       <c r="F59" s="15"/>
       <c r="G59" s="15"/>
@@ -9773,7 +9767,7 @@
       <c r="AF59" s="15"/>
       <c r="AG59" s="15"/>
     </row>
-    <row r="60" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="60" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E60" s="15"/>
       <c r="F60" s="15"/>
       <c r="G60" s="15"/>
@@ -9804,7 +9798,7 @@
       <c r="AF60" s="15"/>
       <c r="AG60" s="15"/>
     </row>
-    <row r="61" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="61" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E61" s="15"/>
       <c r="F61" s="15"/>
       <c r="G61" s="15"/>
@@ -9835,7 +9829,7 @@
       <c r="AF61" s="15"/>
       <c r="AG61" s="15"/>
     </row>
-    <row r="62" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="62" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E62" s="15"/>
       <c r="F62" s="15"/>
       <c r="G62" s="15"/>
@@ -9866,7 +9860,7 @@
       <c r="AF62" s="15"/>
       <c r="AG62" s="15"/>
     </row>
-    <row r="63" spans="5:33" x14ac:dyDescent="0.3">
+    <row r="63" spans="5:33" x14ac:dyDescent="0.45">
       <c r="E63" s="15"/>
       <c r="F63" s="15"/>
       <c r="G63" s="15"/>

</xml_diff>

<commit_message>
Include new technologies in modal share constraints
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_Demand.xlsx
+++ b/SuppXLS/Scen_TRA_Demand.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F677EC0-8A04-4B6B-9F7E-6E7A055D23D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C5E2BF-C85F-4397-BB55-3378C24B954A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="96">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -4299,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B6:AO75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AM7" sqref="AM7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4831,8 +4831,8 @@
         <v>74</v>
       </c>
       <c r="E15" t="str">
-        <f>[1]Commodities!$K$11</f>
-        <v>TMOT_GSL_00</v>
+        <f>LEFT([1]Commodities!$K$11,4)&amp;"*"</f>
+        <v>TMOT*</v>
       </c>
       <c r="H15" t="str">
         <f>H13</f>
@@ -5354,8 +5354,8 @@
         <v>77</v>
       </c>
       <c r="E21" t="str">
-        <f>[1]Commodities!$K$27</f>
-        <v>TBUS_ICE_DST_00</v>
+        <f>LEFT([1]Commodities!$K$27,4)&amp;"*"</f>
+        <v>TBUS*</v>
       </c>
       <c r="H21" t="str">
         <f>H19</f>
@@ -5529,8 +5529,8 @@
         <v>93</v>
       </c>
       <c r="E23" t="str">
-        <f>[1]Commodities!$K$29</f>
-        <v>TLRAIL_ELC_00</v>
+        <f>LEFT([1]Commodities!$K$29,5)&amp;"*"</f>
+        <v>TLRAI*</v>
       </c>
       <c r="H23" t="str">
         <f>H21</f>
@@ -6019,7 +6019,7 @@
         <v>79</v>
       </c>
       <c r="E35" t="str">
-        <f>[1]Commodities!$K$8</f>
+        <f>E11</f>
         <v>TWLK_WLK</v>
       </c>
       <c r="H35" t="str">
@@ -6195,7 +6195,7 @@
         <v>80</v>
       </c>
       <c r="E37" t="str">
-        <f>[1]Commodities!$K$9</f>
+        <f t="shared" ref="E36:E49" si="2">E13</f>
         <v>TCYC_CYC</v>
       </c>
       <c r="H37" t="str">
@@ -6371,8 +6371,8 @@
         <v>81</v>
       </c>
       <c r="E39" t="str">
-        <f>[1]Commodities!$K$11</f>
-        <v>TMOT_GSL_00</v>
+        <f t="shared" si="2"/>
+        <v>TMOT*</v>
       </c>
       <c r="H39" t="str">
         <f>H37</f>
@@ -6546,8 +6546,9 @@
       <c r="C41" t="s">
         <v>82</v>
       </c>
-      <c r="E41" t="s">
-        <v>70</v>
+      <c r="E41" t="str">
+        <f t="shared" si="2"/>
+        <v>TCAR*</v>
       </c>
       <c r="H41" t="str">
         <f>H39</f>
@@ -6721,8 +6722,9 @@
       <c r="C43" t="s">
         <v>83</v>
       </c>
-      <c r="E43" t="s">
-        <v>71</v>
+      <c r="E43" t="str">
+        <f t="shared" si="2"/>
+        <v>TTAXI*</v>
       </c>
       <c r="H43" t="str">
         <f>H41</f>
@@ -6897,8 +6899,8 @@
         <v>84</v>
       </c>
       <c r="E45" t="str">
-        <f>[1]Commodities!$K$27</f>
-        <v>TBUS_ICE_DST_00</v>
+        <f t="shared" si="2"/>
+        <v>TBUS*</v>
       </c>
       <c r="H45" t="str">
         <f>H43</f>
@@ -7073,8 +7075,8 @@
         <v>93</v>
       </c>
       <c r="E47" t="str">
-        <f>[1]Commodities!$K$29</f>
-        <v>TLRAIL_ELC_00</v>
+        <f t="shared" si="2"/>
+        <v>TLRAI*</v>
       </c>
       <c r="H47" t="str">
         <f>H45</f>
@@ -7249,13 +7251,14 @@
         <v>85</v>
       </c>
       <c r="D49" s="32"/>
-      <c r="E49" s="32" t="s">
-        <v>72</v>
+      <c r="E49" t="str">
+        <f t="shared" si="2"/>
+        <v>THRAIL*</v>
       </c>
       <c r="F49" s="32"/>
       <c r="G49" s="32"/>
       <c r="H49" s="32" t="str">
-        <f t="shared" ref="H49" si="2">H47</f>
+        <f t="shared" ref="H49" si="3">H47</f>
         <v>TRAPM</v>
       </c>
       <c r="I49" s="32"/>
@@ -7269,7 +7272,7 @@
         <v>-1</v>
       </c>
       <c r="M49" s="32" t="str">
-        <f t="shared" ref="M49" si="3">M25</f>
+        <f t="shared" ref="M49" si="4">M25</f>
         <v>Train</v>
       </c>
       <c r="N49" s="33">
@@ -7484,107 +7487,107 @@
         <v>*National</v>
       </c>
       <c r="O59" s="5" t="str">
-        <f t="shared" ref="O59:AN59" si="4">O34</f>
+        <f t="shared" ref="O59:AN59" si="5">O34</f>
         <v>IE-CW</v>
       </c>
       <c r="P59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-D</v>
       </c>
       <c r="Q59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-KE</v>
       </c>
       <c r="R59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-KK</v>
       </c>
       <c r="S59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-LS</v>
       </c>
       <c r="T59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-LD</v>
       </c>
       <c r="U59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-LH</v>
       </c>
       <c r="V59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-MH</v>
       </c>
       <c r="W59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-OY</v>
       </c>
       <c r="X59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-WH</v>
       </c>
       <c r="Y59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-WX</v>
       </c>
       <c r="Z59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-WW</v>
       </c>
       <c r="AA59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-CE</v>
       </c>
       <c r="AB59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-CO</v>
       </c>
       <c r="AC59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-KY</v>
       </c>
       <c r="AD59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-LK</v>
       </c>
       <c r="AE59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-TA</v>
       </c>
       <c r="AF59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-WD</v>
       </c>
       <c r="AG59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-G</v>
       </c>
       <c r="AH59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-LM</v>
       </c>
       <c r="AI59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-MO</v>
       </c>
       <c r="AJ59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-RN</v>
       </c>
       <c r="AK59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-SO</v>
       </c>
       <c r="AL59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-CN</v>
       </c>
       <c r="AM59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-DL</v>
       </c>
       <c r="AN59" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>IE-MN</v>
       </c>
       <c r="AO59" s="5" t="s">
@@ -7597,7 +7600,7 @@
       </c>
       <c r="D60" s="34"/>
       <c r="E60" s="34" t="str">
-        <f>[1]Commodities!$K$8</f>
+        <f>E35</f>
         <v>TWLK_WLK</v>
       </c>
       <c r="F60" s="34"/>
@@ -7786,7 +7789,7 @@
       </c>
       <c r="D62" s="34"/>
       <c r="E62" s="34" t="str">
-        <f>[1]Commodities!$K$9</f>
+        <f t="shared" ref="E61:E74" si="6">E37</f>
         <v>TCYC_CYC</v>
       </c>
       <c r="F62" s="34"/>
@@ -7975,8 +7978,8 @@
       </c>
       <c r="D64" s="34"/>
       <c r="E64" s="34" t="str">
-        <f>[1]Commodities!$K$11</f>
-        <v>TMOT_GSL_00</v>
+        <f t="shared" si="6"/>
+        <v>TMOT*</v>
       </c>
       <c r="F64" s="34"/>
       <c r="G64" s="34"/>
@@ -8163,8 +8166,9 @@
         <v>89</v>
       </c>
       <c r="D66" s="34"/>
-      <c r="E66" s="34" t="s">
-        <v>70</v>
+      <c r="E66" s="34" t="str">
+        <f t="shared" si="6"/>
+        <v>TCAR*</v>
       </c>
       <c r="F66" s="34"/>
       <c r="G66" s="34"/>
@@ -8351,8 +8355,9 @@
         <v>90</v>
       </c>
       <c r="D68" s="34"/>
-      <c r="E68" s="34" t="s">
-        <v>71</v>
+      <c r="E68" s="34" t="str">
+        <f t="shared" si="6"/>
+        <v>TTAXI*</v>
       </c>
       <c r="F68" s="34"/>
       <c r="G68" s="34"/>
@@ -8540,8 +8545,8 @@
       </c>
       <c r="D70" s="34"/>
       <c r="E70" s="34" t="str">
-        <f>[1]Commodities!$K$27</f>
-        <v>TBUS_ICE_DST_00</v>
+        <f t="shared" si="6"/>
+        <v>TBUS*</v>
       </c>
       <c r="F70" s="34"/>
       <c r="G70" s="34"/>
@@ -8729,8 +8734,8 @@
       </c>
       <c r="D72" s="34"/>
       <c r="E72" s="34" t="str">
-        <f>[1]Commodities!$K$29</f>
-        <v>TLRAIL_ELC_00</v>
+        <f t="shared" si="6"/>
+        <v>TLRAI*</v>
       </c>
       <c r="F72" s="34"/>
       <c r="G72" s="34"/>
@@ -8916,13 +8921,14 @@
         <v>92</v>
       </c>
       <c r="D74" s="32"/>
-      <c r="E74" s="32" t="s">
-        <v>72</v>
+      <c r="E74" s="34" t="str">
+        <f t="shared" si="6"/>
+        <v>THRAIL*</v>
       </c>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
       <c r="H74" s="32" t="str">
-        <f t="shared" ref="H74" si="5">H72</f>
+        <f t="shared" ref="H74" si="7">H72</f>
         <v>TRAPL</v>
       </c>
       <c r="I74" s="32"/>
@@ -8936,7 +8942,7 @@
         <v>-1</v>
       </c>
       <c r="M74" s="32" t="str">
-        <f t="shared" ref="M74" si="6">M49</f>
+        <f t="shared" ref="M74" si="8">M49</f>
         <v>Train</v>
       </c>
       <c r="N74" s="33">

</xml_diff>